<commit_message>
draft layout, fix footprints
</commit_message>
<xml_diff>
--- a/EdisonBlock_915MHz_fab/EdisonBlock_915MHz_mfg_BoM.xlsx
+++ b/EdisonBlock_915MHz_fab/EdisonBlock_915MHz_mfg_BoM.xlsx
@@ -12,7 +12,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="EdisonBlock_915MHz" localSheetId="0">Sheet1!$A$1:$G$45</definedName>
+    <definedName name="EdisonBlock_915MHz" localSheetId="0">Sheet1!$A$1:$G$46</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="150">
   <si>
     <t>Id</t>
   </si>
@@ -94,9 +94,6 @@
     <t>SW_SPDT_PCM12</t>
   </si>
   <si>
-    <t>CUS-12TB</t>
-  </si>
-  <si>
     <t>U4</t>
   </si>
   <si>
@@ -373,9 +370,6 @@
     <t>H124603CT-ND</t>
   </si>
   <si>
-    <t>563-1102-1-ND</t>
-  </si>
-  <si>
     <t>296-38889-1-ND</t>
   </si>
   <si>
@@ -479,6 +473,21 @@
   </si>
   <si>
     <t>C13,C1,C2,C15,C16,C24,C28</t>
+  </si>
+  <si>
+    <t>B3U-1000P</t>
+  </si>
+  <si>
+    <t>SW1020CT-ND</t>
+  </si>
+  <si>
+    <t>A2</t>
+  </si>
+  <si>
+    <t>A118077CT-ND</t>
+  </si>
+  <si>
+    <t>1909763-1</t>
   </si>
 </sst>
 </file>
@@ -535,7 +544,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -548,6 +557,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -853,10 +866,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G45"/>
+  <dimension ref="A1:G46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:A45"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -884,13 +897,13 @@
         <v>3</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F1" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="G1" s="4" t="s">
         <v>84</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -898,206 +911,203 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>83</v>
-      </c>
       <c r="D2" s="3">
         <v>1</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F2" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
+    </row>
+    <row r="3" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2"/>
+      <c r="B3" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="D3" s="3">
+        <v>1</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
         <f>A2+1</f>
         <v>2</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="D3" s="3">
+      <c r="B4" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D4" s="3">
         <v>2</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E4" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>108</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
-        <f>A3+1</f>
-        <v>3</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D4" s="3">
-        <v>7</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="5" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <f>A4+1</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>80</v>
+        <v>144</v>
       </c>
       <c r="C5" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="3">
+        <v>7</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="3">
-        <v>1</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>81</v>
-      </c>
       <c r="F5" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>88</v>
+        <v>142</v>
       </c>
     </row>
     <row r="6" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <f>A5+1</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D6" s="3">
         <v>1</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>119</v>
+        <v>87</v>
       </c>
     </row>
     <row r="7" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <f>A6+1</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>46</v>
+        <v>25</v>
       </c>
       <c r="D7" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>99</v>
+        <v>117</v>
       </c>
     </row>
     <row r="8" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
-        <f t="shared" ref="A8:A45" si="0">A7+1</f>
-        <v>7</v>
+        <f>A7+1</f>
+        <v>6</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>145</v>
+        <v>73</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>26</v>
+        <v>45</v>
       </c>
       <c r="D8" s="3">
         <v>2</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="G8" s="1"/>
+        <v>74</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="9" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
-        <f t="shared" si="0"/>
-        <v>8</v>
+        <f t="shared" ref="A9:A46" si="0">A8+1</f>
+        <v>7</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>45</v>
+        <v>143</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>46</v>
+        <v>25</v>
       </c>
       <c r="D9" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>103</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="G9" s="1"/>
     </row>
     <row r="10" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>134</v>
+        <v>44</v>
       </c>
       <c r="C10" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D10" s="3">
+        <v>1</v>
+      </c>
+      <c r="E10" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="D10" s="3">
-        <v>5</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>54</v>
-      </c>
       <c r="F10" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>102</v>
@@ -1106,332 +1116,332 @@
     <row r="11" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>48</v>
+        <v>132</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D11" s="3">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>34</v>
+        <v>53</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="12" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D12" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="13" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D13" s="3">
         <v>1</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="14" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <f t="shared" si="0"/>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>28</v>
+        <v>50</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>29</v>
+        <v>45</v>
       </c>
       <c r="D14" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>30</v>
+        <v>51</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="15" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>131</v>
+        <v>27</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>132</v>
+        <v>28</v>
       </c>
       <c r="D15" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>139</v>
+        <v>29</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>138</v>
+        <v>111</v>
       </c>
     </row>
     <row r="16" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>40</v>
+        <v>129</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>41</v>
+        <v>130</v>
       </c>
       <c r="D16" s="3">
         <v>1</v>
       </c>
-      <c r="E16" s="5" t="s">
-        <v>114</v>
+      <c r="E16" s="3" t="s">
+        <v>137</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>115</v>
+        <v>136</v>
       </c>
     </row>
     <row r="17" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>7</v>
+        <v>39</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="D17" s="3">
         <v>1</v>
       </c>
-      <c r="E17" s="3" t="s">
-        <v>9</v>
+      <c r="E17" s="5" t="s">
+        <v>112</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="18" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <f t="shared" si="0"/>
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>31</v>
+        <v>7</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>122</v>
+        <v>8</v>
       </c>
       <c r="D18" s="3">
         <v>1</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>32</v>
+        <v>9</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
     </row>
     <row r="19" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <f t="shared" si="0"/>
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D19" s="3">
         <v>1</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="20" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>72</v>
+        <v>32</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="D20" s="3">
         <v>1</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>73</v>
+        <v>33</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
     </row>
     <row r="21" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>4</v>
+        <v>71</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>5</v>
+        <v>126</v>
       </c>
       <c r="D21" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>6</v>
+        <v>72</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="22" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <f t="shared" si="0"/>
-        <v>21</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="D22" s="4">
-        <v>1</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="G22" s="4"/>
+        <v>20</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D22" s="3">
+        <v>2</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="23" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <f t="shared" si="0"/>
-        <v>22</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D23" s="3">
-        <v>3</v>
-      </c>
-      <c r="E23" s="3">
-        <v>330</v>
-      </c>
-      <c r="F23" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>94</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="D23" s="4">
+        <v>1</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="G23" s="4"/>
     </row>
     <row r="24" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <f t="shared" si="0"/>
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D24" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E24" s="3">
-        <v>287</v>
+        <v>330</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G24" s="1" t="s">
         <v>93</v>
@@ -1440,46 +1450,46 @@
     <row r="25" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <f t="shared" si="0"/>
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D25" s="3">
         <v>1</v>
       </c>
-      <c r="E25" s="3" t="s">
-        <v>68</v>
+      <c r="E25" s="3">
+        <v>287</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="26" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <f t="shared" si="0"/>
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D26" s="3">
-        <v>2</v>
-      </c>
-      <c r="E26" s="3">
-        <v>100</v>
+        <v>1</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>67</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G26" s="1" t="s">
         <v>90</v>
@@ -1488,446 +1498,470 @@
     <row r="27" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <f t="shared" si="0"/>
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D27" s="3">
         <v>2</v>
       </c>
       <c r="E27" s="3">
-        <v>27</v>
+        <v>100</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="28" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D28" s="3">
+        <v>2</v>
+      </c>
+      <c r="E28" s="3">
         <v>27</v>
       </c>
-      <c r="B28" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D28" s="3">
-        <v>1</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>58</v>
-      </c>
       <c r="F28" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="29" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <f t="shared" si="0"/>
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D29" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>60</v>
+        <v>57</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="30" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <f t="shared" si="0"/>
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D30" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="F30" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="G30" s="1" t="s">
-        <v>96</v>
+        <v>59</v>
       </c>
     </row>
     <row r="31" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <f t="shared" si="0"/>
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D31" s="3">
         <v>1</v>
       </c>
-      <c r="E31" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="F31" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="G31" s="7" t="s">
-        <v>97</v>
+      <c r="E31" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="32" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <f t="shared" si="0"/>
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>140</v>
+        <v>62</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D32" s="3">
-        <v>2</v>
-      </c>
-      <c r="E32" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="F32" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="G32" s="1" t="s">
-        <v>98</v>
+        <v>1</v>
+      </c>
+      <c r="E32" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="F32" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="G32" s="7" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="33" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <f t="shared" si="0"/>
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>16</v>
+        <v>138</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>17</v>
+        <v>55</v>
       </c>
       <c r="D33" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>18</v>
+        <v>64</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>111</v>
+        <v>97</v>
       </c>
     </row>
     <row r="34" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <f t="shared" si="0"/>
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="D34" s="3">
         <v>1</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>12</v>
+        <v>145</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="G34" s="1" t="s">
-        <v>110</v>
+        <v>85</v>
+      </c>
+      <c r="G34" s="8" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="35" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <f t="shared" si="0"/>
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>77</v>
+        <v>10</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>78</v>
+        <v>11</v>
       </c>
       <c r="D35" s="3">
         <v>1</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>79</v>
+        <v>12</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>89</v>
+        <v>109</v>
       </c>
     </row>
     <row r="36" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <f t="shared" si="0"/>
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>133</v>
+        <v>76</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>36</v>
+        <v>77</v>
       </c>
       <c r="D36" s="3">
         <v>1</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>60</v>
+        <v>78</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>125</v>
+        <v>85</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>125</v>
+        <v>88</v>
       </c>
     </row>
     <row r="37" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <f t="shared" si="0"/>
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D37" s="3">
         <v>1</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="G37" s="1"/>
+        <v>59</v>
+      </c>
+      <c r="F37" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="38" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <f t="shared" si="0"/>
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>13</v>
+        <v>131</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>14</v>
+        <v>35</v>
       </c>
       <c r="D38" s="3">
         <v>1</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F38" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="G38" s="1" t="s">
-        <v>143</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="G38" s="1"/>
     </row>
     <row r="39" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <f t="shared" si="0"/>
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="D39" s="3">
         <v>1</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>112</v>
+        <v>141</v>
       </c>
     </row>
     <row r="40" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <f t="shared" si="0"/>
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>38</v>
+        <v>19</v>
       </c>
       <c r="D40" s="3">
         <v>1</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>39</v>
+        <v>20</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
     </row>
     <row r="41" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <f t="shared" si="0"/>
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>129</v>
+        <v>37</v>
       </c>
       <c r="D41" s="3">
         <v>1</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>129</v>
+        <v>38</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="G41" s="5" t="s">
-        <v>130</v>
+        <v>85</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="42" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <f t="shared" si="0"/>
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>36</v>
+        <v>127</v>
       </c>
       <c r="D42" s="3">
         <v>1</v>
       </c>
-      <c r="E42" s="5" t="s">
-        <v>135</v>
+      <c r="E42" s="3" t="s">
+        <v>127</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="G42" s="1" t="s">
-        <v>136</v>
+        <v>85</v>
+      </c>
+      <c r="G42" s="5" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="43" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <f t="shared" si="0"/>
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="D43" s="3">
         <v>1</v>
       </c>
-      <c r="E43" s="3" t="s">
-        <v>44</v>
+      <c r="E43" s="5" t="s">
+        <v>133</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>101</v>
+        <v>134</v>
       </c>
     </row>
     <row r="44" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
         <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D44" s="3">
+        <v>1</v>
+      </c>
+      <c r="E44" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B44" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="C44" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="D44" s="3">
-        <v>1</v>
-      </c>
-      <c r="E44" s="3" t="s">
-        <v>141</v>
-      </c>
       <c r="F44" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>142</v>
+        <v>100</v>
       </c>
     </row>
     <row r="45" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <f t="shared" si="0"/>
+        <v>43</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="D45" s="3">
+        <v>1</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="F45" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="2">
+        <f t="shared" si="0"/>
         <v>44</v>
       </c>
-      <c r="B45" s="3" t="s">
+      <c r="B46" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C46" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C45" s="3" t="s">
+      <c r="D46" s="3">
+        <v>1</v>
+      </c>
+      <c r="E46" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D45" s="3">
-        <v>1</v>
-      </c>
-      <c r="E45" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="F45" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="G45" s="1" t="s">
-        <v>107</v>
+      <c r="F46" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>106</v>
       </c>
     </row>
   </sheetData>

</xml_diff>